<commit_message>
modificacion frmoulario de venta con multiples formas de pago
</commit_message>
<xml_diff>
--- a/Plantilla/TemplateProductoSucursal.xlsx
+++ b/Plantilla/TemplateProductoSucursal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tambours\OneDrive - Hewlett Packard Enterprise\Personal\Desarrollo\Repos\Cinderella\Plantilla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stambour\OneDrive - DXC Production\Personal\Desarrollo\Repos\Cinderella\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -186,25 +186,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,13 +482,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="1" max="2" width="9.140625" style="12"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="62.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
@@ -543,52 +538,41 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="9"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="13"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:L1"/>
-  <dataValidations count="10">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El código ingresado ya se encuentra utilizado." sqref="C2:C3">
-      <formula1>COUNTIF(C:C,$D2)=1</formula1>
-    </dataValidation>
+  <dataConsolidate/>
+  <dataValidations count="6">
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El origen ingresado no debe estar vacío y debe ser menor a los 255 caracteres." sqref="G1"/>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El Nombre ingresado no debe estar vacío y debe ser menor a los 255 caracteres." sqref="D2:D3 C1">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El Nombre ingresado no debe estar vacío y debe ser menor a los 255 caracteres." sqref="C1">
       <formula1>1</formula1>
       <formula2>255</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
-      <formula1>INDIRECT(SUBSTITUTE($F2," ","_"))</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3">
-      <formula1>Porveedores</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
-      <formula1>Categorias</formula1>
     </dataValidation>
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El código barras ingresado no debe estar vacío y debe tener 13 dígitos." sqref="K2:K3">
       <formula1>1000000000000</formula1>

</xml_diff>

<commit_message>
Agregado de exportar e importar excel base para productos y stock
</commit_message>
<xml_diff>
--- a/Plantilla/TemplateProductoSucursal.xlsx
+++ b/Plantilla/TemplateProductoSucursal.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stambour\OneDrive - DXC Production\Personal\Desarrollo\Repos\Cinderella\Plantilla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/santiago_tambour_dxc_com/Documents/Personal/Desarrollo/Repos/Cinderella/Plantilla/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_C5462684364C43007836B02818B7EB25158CE384" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97DEB4D4-E074-4925-BCBE-6A6FAE83EDA0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10485"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Codigo</t>
   </si>
@@ -61,14 +62,17 @@
     <t>VentaMensual</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>id_producto</t>
+  </si>
+  <si>
+    <t>id_Stock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +88,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,8 +127,19 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -182,11 +204,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -200,8 +249,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,16 +534,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="12"/>
+    <col min="1" max="2" width="0" style="12" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="62.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
@@ -502,11 +557,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -539,9 +596,9 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -554,7 +611,7 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -566,28 +623,26 @@
       <c r="L3" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:L1"/>
+  <autoFilter ref="C1:L1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataConsolidate/>
-  <dataValidations count="6">
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El origen ingresado no debe estar vacío y debe ser menor a los 255 caracteres." sqref="G1"/>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El Nombre ingresado no debe estar vacío y debe ser menor a los 255 caracteres." sqref="C1">
+  <dataValidations count="5">
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El origen ingresado no debe estar vacío y debe ser menor a los 255 caracteres." sqref="G1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El Nombre ingresado no debe estar vacío y debe ser menor a los 255 caracteres." sqref="C1" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
       <formula2>255</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El código barras ingresado no debe estar vacío y debe tener 13 dígitos." sqref="K2:K3">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Valore ingresado incorrecto" error="El código barras ingresado no debe estar vacío y debe tener 13 dígitos." sqref="K2:K3" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>1000000000000</formula1>
       <formula2>9999999999999</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Solo se pueden ingresar valores enteros mayores o iguales a 0" sqref="J1:J1048576">
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Solo se pueden ingresar valores enteros mayores o iguales a 0" sqref="J1:J1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>-1</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Solo se pueden ingresar valores enteros mayores o iguales a 0" sqref="H1:H1048576 I1:I1048576">
-      <formula1>-1</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Solo se pueden ingresar valores enteros mayores o iguales a 0" sqref="L1:L1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Solo se pueden ingresar valores enteros mayores o iguales a 0" sqref="H1:I1048576 L1:L1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>-1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>